<commit_message>
Eerste extra paper toegevoegd, zonder comments
</commit_message>
<xml_diff>
--- a/Papers/Overview Papers.xlsx
+++ b/Papers/Overview Papers.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piete\OneDrive\Documents\GitHub\Microsoft\Papers\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Toon Stolk\Documents\Education\Space Engineering\Courses\Microsat Engineering\GitHub Repository\Microsoft\Papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E0B8EB-5693-4CDF-9ACB-CDD6C4CFDDAA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE781EAB-5D2C-4FF9-874F-11F982EE9C7C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Paper Name</t>
   </si>
@@ -43,6 +43,9 @@
   </si>
   <si>
     <t>setup on how to make the filter</t>
+  </si>
+  <si>
+    <t>Review of the Robustness and Applicability of Monocular Pose Estimation Systems for Relative Navigation with an Uncooperative Spacecraft</t>
   </si>
 </sst>
 </file>
@@ -360,7 +363,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
@@ -368,7 +371,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="42" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="116.109375" customWidth="1"/>
     <col min="2" max="2" width="16.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
@@ -395,6 +398,11 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>